<commit_message>
Wheelchair - started developing the motor driver code. Hardware - updated BOMs.
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="19155" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -158,12 +158,6 @@
     <t>712-1420-1-ND</t>
   </si>
   <si>
-    <t>Newark</t>
-  </si>
-  <si>
-    <t>42M2397</t>
-  </si>
-  <si>
     <t>Nordic Wireless</t>
   </si>
   <si>
@@ -272,24 +266,12 @@
     <t>L-07C8N2JV6T</t>
   </si>
   <si>
-    <t>NRF24L01G</t>
-  </si>
-  <si>
     <t>Nordic Semiconductor</t>
   </si>
   <si>
     <t>IC2</t>
   </si>
   <si>
-    <t>ATTINY261V-10MU</t>
-  </si>
-  <si>
-    <t>ATTINY261V-10MU-ND</t>
-  </si>
-  <si>
-    <t>Attiny26 microcontroller QFN32</t>
-  </si>
-  <si>
     <t>Atmel</t>
   </si>
   <si>
@@ -429,6 +411,24 @@
   </si>
   <si>
     <t>C1005C0G1H1R5B</t>
+  </si>
+  <si>
+    <t>Attiny461 microcontroller QFN32</t>
+  </si>
+  <si>
+    <t>ATTINY461V-10MURCT-ND</t>
+  </si>
+  <si>
+    <t>ATTINY461V-10MUR</t>
+  </si>
+  <si>
+    <t>nRF24L01P-T</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>949-NRF24L01P-T</t>
   </si>
 </sst>
 </file>
@@ -1703,8 +1703,8 @@
   </sheetPr>
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1714,7 @@
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" style="32" bestFit="1" customWidth="1"/>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>175.37</v>
+        <v>173.66</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>39</v>
@@ -1813,7 +1813,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" s="11">
         <v>0.04</v>
@@ -1833,10 +1833,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>38</v>
@@ -1848,7 +1848,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" s="11">
         <v>0.06</v>
@@ -1868,22 +1868,22 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H6" s="29">
         <v>0.02</v>
@@ -1903,22 +1903,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" s="29">
         <v>0.02</v>
@@ -1972,22 +1972,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H10" s="18">
         <v>0.16</v>
@@ -2007,10 +2007,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>17</v>
@@ -2042,10 +2042,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>19</v>
@@ -2077,10 +2077,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>22</v>
@@ -2112,10 +2112,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>25</v>
@@ -2147,10 +2147,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>30</v>
@@ -2159,7 +2159,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>28</v>
@@ -2182,10 +2182,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>29</v>
@@ -2194,7 +2194,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>31</v>
@@ -2217,10 +2217,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>32</v>
@@ -2229,7 +2229,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>33</v>
@@ -2252,10 +2252,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>35</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -2321,10 +2321,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>41</v>
@@ -2336,7 +2336,7 @@
         <v>42</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H21" s="24">
         <v>0.05</v>
@@ -2356,10 +2356,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>43</v>
@@ -2371,7 +2371,7 @@
         <v>44</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H22" s="24">
         <v>0.05</v>
@@ -2391,10 +2391,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>45</v>
@@ -2406,7 +2406,7 @@
         <v>46</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H23" s="24">
         <v>0.05</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -2460,32 +2460,32 @@
         <v>17</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H26" s="24">
-        <v>2.8</v>
+        <v>3.05</v>
       </c>
       <c r="I26" s="10">
         <v>1</v>
       </c>
       <c r="J26" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.8</v>
+        <v>3.05</v>
       </c>
       <c r="K26" s="13"/>
     </row>
@@ -2495,32 +2495,32 @@
         <v>18</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H27" s="24">
-        <v>5.56</v>
+        <v>3.6</v>
       </c>
       <c r="I27" s="12">
         <v>1</v>
       </c>
       <c r="J27" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>5.56</v>
+        <v>3.6</v>
       </c>
       <c r="K27" s="22"/>
     </row>
@@ -2564,22 +2564,22 @@
         <v>19</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H30" s="11">
         <v>2.36</v>
@@ -2599,22 +2599,22 @@
         <v>20</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C31" s="10">
         <v>3003</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H31" s="11">
         <v>0.65</v>
@@ -2634,22 +2634,22 @@
         <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H32" s="11">
         <v>0.26</v>
@@ -2669,22 +2669,22 @@
         <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H33" s="11">
         <v>3.5</v>
@@ -2704,22 +2704,22 @@
         <v>23</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H34" s="11">
         <v>4.95</v>
@@ -2739,22 +2739,22 @@
         <v>24</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H35" s="11">
         <v>0.13</v>
@@ -2774,11 +2774,11 @@
         <v>25</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="34" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -2801,19 +2801,19 @@
         <v>26</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="D37" s="34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E37" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="11">
@@ -2834,19 +2834,19 @@
         <v>27</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="11">
@@ -2954,12 +2954,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -2968,15 +2968,15 @@
         <v>7</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2989,7 +2989,7 @@
         <v>150</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote schematic - changed thumb joystick. Circuit design checkpoint.
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
   <si>
     <t>ID #</t>
   </si>
@@ -194,15 +194,6 @@
     <t>RMCF0402JT220RCT-ND</t>
   </si>
   <si>
-    <t>Polycase</t>
-  </si>
-  <si>
-    <t>Case, Black ABS, 3.52 x 1.77 x 0.73 in</t>
-  </si>
-  <si>
-    <t>KT-45T0 </t>
-  </si>
-  <si>
     <t>UMK105CG220JV-F</t>
   </si>
   <si>
@@ -290,15 +281,6 @@
     <t>XTAL1</t>
   </si>
   <si>
-    <t>3003K-ND</t>
-  </si>
-  <si>
-    <t>Battery Holder 20mm Coin Cell</t>
-  </si>
-  <si>
-    <t>Keystone</t>
-  </si>
-  <si>
     <t>BAT1</t>
   </si>
   <si>
@@ -332,33 +314,12 @@
     <t>JP1</t>
   </si>
   <si>
-    <t>COM-09426</t>
-  </si>
-  <si>
     <t>Sparkfun</t>
   </si>
   <si>
-    <t>Thumbstick PSP style</t>
-  </si>
-  <si>
     <t>JSTICK1</t>
   </si>
   <si>
-    <t>COM-08996</t>
-  </si>
-  <si>
-    <t>Mini button pad set Red</t>
-  </si>
-  <si>
-    <t>U3-U10</t>
-  </si>
-  <si>
-    <t>Paul Shields</t>
-  </si>
-  <si>
-    <t>Light Pipe 0603</t>
-  </si>
-  <si>
     <t>Other Circuit Costs</t>
   </si>
   <si>
@@ -429,6 +390,30 @@
   </si>
   <si>
     <t>949-NRF24L01P-T</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TPS61200DRCT</t>
+  </si>
+  <si>
+    <t>Boost regulator</t>
+  </si>
+  <si>
+    <t>296-21663-1-ND</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>Battery Holder AAA</t>
+  </si>
+  <si>
+    <t>Thumb Joystick PS2 style</t>
+  </si>
+  <si>
+    <t>Button</t>
   </si>
 </sst>
 </file>
@@ -438,7 +423,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,8 +625,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,18 +810,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -994,7 +973,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1083,19 +1062,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1388,8 +1370,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K39" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K40" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K40"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID #" dataDxfId="10">
       <calculatedColumnFormula>1+A2</calculatedColumnFormula>
@@ -1701,10 +1683,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,7 +1718,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>173.66</v>
+        <v>164.79</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -1803,7 +1785,7 @@
       <c r="C4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -1813,7 +1795,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H4" s="11">
         <v>0.04</v>
@@ -1838,7 +1820,7 @@
       <c r="C5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -1848,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5" s="11">
         <v>0.06</v>
@@ -1873,7 +1855,7 @@
       <c r="C6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="39" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="10" t="s">
@@ -1883,7 +1865,7 @@
         <v>56</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6" s="29">
         <v>0.02</v>
@@ -1908,7 +1890,7 @@
       <c r="C7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="39" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -1918,7 +1900,7 @@
         <v>58</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H7" s="29">
         <v>0.02</v>
@@ -1972,22 +1954,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H10" s="18">
         <v>0.16</v>
@@ -2007,12 +1989,12 @@
         <v>6</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="16" t="s">
@@ -2042,12 +2024,12 @@
         <v>7</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2077,12 +2059,12 @@
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="16" t="s">
@@ -2112,12 +2094,12 @@
         <v>9</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="16" t="s">
@@ -2147,19 +2129,19 @@
         <v>10</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>28</v>
@@ -2182,19 +2164,19 @@
         <v>11</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>31</v>
@@ -2217,19 +2199,19 @@
         <v>12</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>33</v>
@@ -2252,12 +2234,12 @@
         <v>13</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -2299,7 +2281,7 @@
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -2321,12 +2303,12 @@
         <v>14</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>41</v>
       </c>
       <c r="E21" s="21" t="s">
@@ -2336,7 +2318,7 @@
         <v>42</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H21" s="24">
         <v>0.05</v>
@@ -2356,12 +2338,12 @@
         <v>15</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="21" t="s">
@@ -2371,7 +2353,7 @@
         <v>44</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H22" s="24">
         <v>0.05</v>
@@ -2391,12 +2373,12 @@
         <v>16</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="21" t="s">
@@ -2406,7 +2388,7 @@
         <v>46</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H23" s="24">
         <v>0.05</v>
@@ -2438,7 +2420,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -2454,96 +2436,113 @@
       </c>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <f>A23+1</f>
         <v>17</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>132</v>
+      <c r="B26" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>133</v>
+      <c r="F26" s="34" t="s">
+        <v>128</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H26" s="24">
-        <v>3.05</v>
-      </c>
-      <c r="I26" s="10">
+        <v>129</v>
+      </c>
+      <c r="H26" s="35">
+        <v>3.74</v>
+      </c>
+      <c r="I26" s="36">
         <v>1</v>
       </c>
-      <c r="J26" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.05</v>
-      </c>
-      <c r="K26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.74</v>
+      </c>
+      <c r="K26" s="38"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <f>A26+1</f>
         <v>18</v>
       </c>
       <c r="B27" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="D27" s="37" t="s">
+      <c r="H27" s="24">
+        <v>3.05</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.05</v>
+      </c>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <f>A27+1</f>
+        <v>19</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="24">
+      <c r="E28" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" s="24">
         <v>3.6</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I28" s="12">
         <v>1</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J28" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>3.6</v>
       </c>
-      <c r="K27" s="22"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="20"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>13</v>
-      </c>
+      <c r="A29" s="25"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -2559,107 +2558,82 @@
       <c r="K29" s="20"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="25">
-        <f>A27+1</f>
-        <v>19</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="37" t="s">
+      <c r="A30" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <f>A28+1</f>
+        <v>20</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H30" s="11">
-        <v>2.36</v>
-      </c>
-      <c r="I30" s="10">
-        <v>1</v>
-      </c>
-      <c r="J30" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.36</v>
-      </c>
-      <c r="K30" s="13"/>
-    </row>
-    <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25">
-        <f t="shared" ref="A31:A36" si="2">A30+1</f>
-        <v>20</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="10">
-        <v>3003</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>92</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H31" s="11">
-        <v>0.65</v>
-      </c>
-      <c r="I31" s="12">
+        <v>2.36</v>
+      </c>
+      <c r="I31" s="10">
         <v>1</v>
       </c>
       <c r="J31" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.65</v>
+        <v>2.36</v>
       </c>
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A32:A37" si="2">A31+1</f>
         <v>21</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>102</v>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="F32" s="10"/>
       <c r="G32" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="11">
-        <v>0.26</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="H32" s="11"/>
       <c r="I32" s="12">
         <v>1</v>
       </c>
       <c r="J32" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="K32" s="13"/>
     </row>
@@ -2669,32 +2643,32 @@
         <v>22</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>107</v>
+        <v>94</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H33" s="11">
-        <v>3.5</v>
+        <v>0.26</v>
       </c>
       <c r="I33" s="12">
         <v>1</v>
       </c>
       <c r="J33" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.5</v>
+        <v>0.26</v>
       </c>
       <c r="K33" s="13"/>
     </row>
@@ -2704,32 +2678,26 @@
         <v>23</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>110</v>
+        <v>99</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="21" t="s">
+        <v>131</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>109</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F34" s="10"/>
       <c r="G34" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="H34" s="11">
-        <v>4.95</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="H34" s="11"/>
       <c r="I34" s="12">
         <v>1</v>
       </c>
       <c r="J34" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>4.95</v>
+        <v>0</v>
       </c>
       <c r="K34" s="13"/>
     </row>
@@ -2739,32 +2707,24 @@
         <v>24</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" s="11">
-        <v>0.13</v>
-      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="12">
         <v>1</v>
       </c>
       <c r="J35" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="K35" s="13"/>
     </row>
@@ -2774,126 +2734,138 @@
         <v>25</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+        <v>92</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="H36" s="11">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I36" s="12">
         <v>1</v>
       </c>
       <c r="J36" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
-        <f>A36+1</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="11">
-        <v>3.51</v>
-      </c>
+      <c r="H37" s="11"/>
       <c r="I37" s="12">
         <v>1</v>
       </c>
       <c r="J37" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.51</v>
+        <v>0</v>
       </c>
       <c r="K37" s="13"/>
     </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
-        <f>1+A37</f>
+        <f>A37+1</f>
         <v>27</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>123</v>
-      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="11">
-        <v>150</v>
-      </c>
+      <c r="H38" s="11"/>
       <c r="I38" s="12">
         <v>1</v>
       </c>
       <c r="J38" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
+        <f>1+A38</f>
+        <v>28</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="11">
         <v>150</v>
       </c>
-      <c r="K38" s="13"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="27"/>
+      <c r="I39" s="12">
+        <v>1</v>
+      </c>
       <c r="J39" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>150</v>
+      </c>
+      <c r="K39" s="13"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K39" s="13"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="K40" s="13"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -2905,7 +2877,8 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
@@ -2913,8 +2886,7 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
@@ -2927,6 +2899,11 @@
       <c r="A53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2954,12 +2931,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -2968,15 +2945,15 @@
         <v>7</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2989,7 +2966,7 @@
         <v>150</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote schematic and routing checkpoint
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="171">
   <si>
     <t>ID #</t>
   </si>
@@ -206,9 +206,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>TMK105BJ104KV-F</t>
   </si>
   <si>
-    <t>0.1uF 0402</t>
-  </si>
-  <si>
     <t>C10</t>
   </si>
   <si>
@@ -398,22 +392,205 @@
     <t>TPS61200DRCT</t>
   </si>
   <si>
-    <t>Boost regulator</t>
-  </si>
-  <si>
     <t>296-21663-1-ND</t>
   </si>
   <si>
     <t>IC3</t>
   </si>
   <si>
-    <t>Battery Holder AAA</t>
-  </si>
-  <si>
     <t>Thumb Joystick PS2 style</t>
   </si>
   <si>
     <t>Button</t>
+  </si>
+  <si>
+    <t>Battery Holder 2xAA</t>
+  </si>
+  <si>
+    <t>COM-09032</t>
+  </si>
+  <si>
+    <t>Adjustable Boost regulator</t>
+  </si>
+  <si>
+    <t>5V Boost regulator</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>TPS61202DSCR</t>
+  </si>
+  <si>
+    <t>296-24865-1-ND</t>
+  </si>
+  <si>
+    <t>3.5mm mono jack female</t>
+  </si>
+  <si>
+    <t>Kobiconn</t>
+  </si>
+  <si>
+    <t>161-1640-EX</t>
+  </si>
+  <si>
+    <t>On/off switch</t>
+  </si>
+  <si>
+    <t>CH864-ND</t>
+  </si>
+  <si>
+    <t>PRK22J5BBBNN</t>
+  </si>
+  <si>
+    <t>Cherry</t>
+  </si>
+  <si>
+    <t>MLZ2012M2R2H</t>
+  </si>
+  <si>
+    <r>
+      <t>2.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H 0805</t>
+    </r>
+  </si>
+  <si>
+    <t>445-8658-1-ND</t>
+  </si>
+  <si>
+    <t>L4, L5</t>
+  </si>
+  <si>
+    <t>75k 0402</t>
+  </si>
+  <si>
+    <t>330k 0402</t>
+  </si>
+  <si>
+    <t>RMCF0402FT75K0</t>
+  </si>
+  <si>
+    <t>RMCF0402FT75K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT330K</t>
+  </si>
+  <si>
+    <t>RMCF0402FT330KCT-ND</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>C1608X5R0J226M</t>
+  </si>
+  <si>
+    <t>445-8028-1-ND</t>
+  </si>
+  <si>
+    <r>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F 0603</t>
+    </r>
+  </si>
+  <si>
+    <t>0.1μF 0402</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F 0402</t>
+    </r>
+  </si>
+  <si>
+    <t>C0402C105K9PACTU</t>
+  </si>
+  <si>
+    <t>399-4873-1-ND</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>C11, C14, C15</t>
+  </si>
+  <si>
+    <t>R3, R7, R8, R9, R10</t>
+  </si>
+  <si>
+    <t>Semtech</t>
+  </si>
+  <si>
+    <t>UCLAMP3304A.TCT</t>
+  </si>
+  <si>
+    <t>3.3V TVS</t>
+  </si>
+  <si>
+    <t>UCLAMP3304ACT-ND</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -423,7 +600,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,6 +807,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -973,7 +1163,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1079,6 +1269,21 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1370,8 +1575,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K40" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K47" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K47"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID #" dataDxfId="10">
       <calculatedColumnFormula>1+A2</calculatedColumnFormula>
@@ -1683,10 +1888,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1923,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>164.79</v>
+        <v>179.74</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -1865,17 +2070,17 @@
         <v>56</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="H6" s="29">
         <v>0.02</v>
       </c>
       <c r="I6" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J6" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="K6" s="13"/>
     </row>
@@ -1900,7 +2105,7 @@
         <v>58</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="29">
         <v>0.02</v>
@@ -1914,167 +2119,167 @@
       </c>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42">
+        <f>1+A7</f>
+        <v>5</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="I8" s="44">
+        <v>1</v>
+      </c>
+      <c r="J8" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.04</v>
+      </c>
+      <c r="K8" s="41"/>
+    </row>
+    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42">
+        <f>1+A8</f>
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" s="37">
+        <v>0.04</v>
+      </c>
+      <c r="I9" s="44">
+        <v>1</v>
+      </c>
+      <c r="J9" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.04</v>
+      </c>
+      <c r="K9" s="41"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11">
+      <c r="B11" s="15"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
-      </c>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <f>A7+1</f>
-        <v>5</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="18">
-        <v>0.16</v>
-      </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.16</v>
-      </c>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <f t="shared" ref="A11:A16" si="0">1+A10</f>
-        <v>6</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="19">
-        <v>0.08</v>
-      </c>
-      <c r="I11" s="10">
-        <v>1</v>
-      </c>
-      <c r="J11" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.08</v>
       </c>
       <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <f t="shared" si="0"/>
+        <f>A9+1</f>
         <v>7</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="16" t="s">
+      <c r="C12" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="19">
-        <v>0.08</v>
+      <c r="F12" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.16</v>
       </c>
       <c r="I12" s="10">
         <v>1</v>
       </c>
       <c r="J12" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.08</v>
-      </c>
-      <c r="K12" s="22"/>
+        <v>0.16</v>
+      </c>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A13:A18" si="0">1+A12</f>
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>22</v>
+      <c r="D13" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>23</v>
+      <c r="F13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="H13" s="19">
         <v>0.08</v>
@@ -2086,7 +2291,7 @@
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.08</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
@@ -2097,29 +2302,29 @@
         <v>60</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="24">
-        <v>0.12</v>
+        <v>21</v>
+      </c>
+      <c r="H14" s="19">
+        <v>0.08</v>
       </c>
       <c r="I14" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="K14" s="22"/>
     </row>
@@ -2129,32 +2334,32 @@
         <v>10</v>
       </c>
       <c r="B15" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>114</v>
-      </c>
       <c r="D15" s="21" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0.12</v>
+        <v>23</v>
+      </c>
+      <c r="H15" s="19">
+        <v>0.08</v>
       </c>
       <c r="I15" s="10">
         <v>1</v>
       </c>
       <c r="J15" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="K15" s="22"/>
     </row>
@@ -2164,62 +2369,62 @@
         <v>11</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H16" s="24">
         <v>0.12</v>
       </c>
       <c r="I16" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <f>1+A16</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H17" s="24">
         <v>0.12</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="10">
         <v>1</v>
       </c>
       <c r="J17" s="11">
@@ -2228,182 +2433,201 @@
       </c>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <f>1+A17</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0.12</v>
+      </c>
+      <c r="I18" s="10">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.12</v>
+      </c>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <f>1+A18</f>
+        <v>14</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0.12</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1</v>
+      </c>
+      <c r="J19" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.12</v>
+      </c>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <f>1+A19</f>
+        <v>15</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H20" s="24">
         <v>0.36</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I20" s="12">
         <v>1</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J20" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.36</v>
-      </c>
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <f>A18+1</f>
-        <v>14</v>
+        <f>1+A20</f>
+        <v>16</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="H21" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I21" s="10">
-        <v>1</v>
+        <v>0.38</v>
+      </c>
+      <c r="I21" s="12">
+        <v>3</v>
       </c>
       <c r="J21" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.05</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <f t="shared" ref="A22:A23" si="1">1+A21</f>
-        <v>15</v>
+        <f>1+A21</f>
+        <v>17</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>75</v>
+        <v>161</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="H22" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I22" s="12">
+        <v>2</v>
       </c>
       <c r="J22" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.05</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K22" s="22"/>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I23" s="10">
-        <v>1</v>
-      </c>
+    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="K23" s="22"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>70</v>
+      </c>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -2411,499 +2635,753 @@
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="10"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
       <c r="K24" s="22"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="10"/>
+    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <f>A22+1</f>
+        <v>18</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
       <c r="J25" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
-        <f>A23+1</f>
-        <v>17</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>126</v>
+      <c r="A26" s="14">
+        <f t="shared" ref="A26:A27" si="1">1+A25</f>
+        <v>19</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="34" t="s">
-        <v>128</v>
+      <c r="F26" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" s="35">
-        <v>3.74</v>
-      </c>
-      <c r="I26" s="36">
+        <v>74</v>
+      </c>
+      <c r="H26" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I26" s="10">
         <v>1</v>
       </c>
-      <c r="J26" s="37">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.74</v>
-      </c>
-      <c r="K26" s="38"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="25">
-        <f>A26+1</f>
-        <v>18</v>
+      <c r="J26" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.05</v>
+      </c>
+      <c r="K26" s="22"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>119</v>
+        <v>77</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H27" s="24">
-        <v>3.05</v>
+        <v>0.05</v>
       </c>
       <c r="I27" s="10">
         <v>1</v>
       </c>
       <c r="J27" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.05</v>
-      </c>
-      <c r="K27" s="13"/>
-    </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
-        <f>A27+1</f>
-        <v>19</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>122</v>
+        <v>0.05</v>
+      </c>
+      <c r="K27" s="22"/>
+    </row>
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="42">
+        <f>1+A27</f>
+        <v>21</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>143</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>124</v>
+        <v>14</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>145</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="H28" s="24">
-        <v>3.6</v>
-      </c>
-      <c r="I28" s="12">
-        <v>1</v>
-      </c>
-      <c r="J28" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.6</v>
-      </c>
-      <c r="K28" s="22"/>
+        <v>146</v>
+      </c>
+      <c r="H28" s="35">
+        <v>0.15</v>
+      </c>
+      <c r="I28" s="36">
+        <v>2</v>
+      </c>
+      <c r="J28" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.3</v>
+      </c>
+      <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="24"/>
       <c r="I29" s="10"/>
       <c r="J29" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K29" s="20"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="19"/>
+        <v>82</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="10"/>
       <c r="J30" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K30" s="20"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <f>A28+1</f>
-        <v>20</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H31" s="11">
-        <v>2.36</v>
+      <c r="F31" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="24">
+        <v>3.05</v>
       </c>
       <c r="I31" s="10">
         <v>1</v>
       </c>
       <c r="J31" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.36</v>
+        <v>3.05</v>
       </c>
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
-        <f t="shared" ref="A32:A37" si="2">A31+1</f>
-        <v>21</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+        <f>A31+1</f>
+        <v>23</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>120</v>
+      </c>
       <c r="D32" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H32" s="11"/>
+        <v>47</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="24">
+        <v>3.6</v>
+      </c>
       <c r="I32" s="12">
         <v>1</v>
       </c>
       <c r="J32" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="13"/>
+        <v>3.6</v>
+      </c>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>94</v>
+        <f>A32+1</f>
+        <v>24</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H33" s="11">
-        <v>0.26</v>
-      </c>
-      <c r="I33" s="12">
+      <c r="F33" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="35">
+        <v>3.74</v>
+      </c>
+      <c r="I33" s="36">
         <v>1</v>
       </c>
-      <c r="J33" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.26</v>
-      </c>
-      <c r="K33" s="13"/>
+      <c r="J33" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.74</v>
+      </c>
+      <c r="K33" s="38"/>
     </row>
     <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="10"/>
+        <f>A33+1</f>
+        <v>25</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="D34" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12">
+        <v>132</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="35">
+        <v>3.17</v>
+      </c>
+      <c r="I34" s="36">
         <v>1</v>
       </c>
       <c r="J34" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.17</v>
+      </c>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K34" s="13"/>
-    </row>
-    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="10" t="s">
+      <c r="K35" s="20"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="25">
+        <f>A34+1</f>
+        <v>26</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12">
+      <c r="F37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" s="11">
+        <v>2.36</v>
+      </c>
+      <c r="I37" s="10">
         <v>1</v>
       </c>
-      <c r="J35" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="13"/>
-    </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H36" s="11">
-        <v>0.13</v>
-      </c>
-      <c r="I36" s="12">
-        <v>1</v>
-      </c>
-      <c r="J36" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.13</v>
-      </c>
-      <c r="K36" s="13"/>
-    </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12">
-        <v>1</v>
-      </c>
       <c r="J37" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>2.36</v>
       </c>
       <c r="K37" s="13"/>
     </row>
     <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
+      <c r="A38" s="40">
         <f>A37+1</f>
         <v>27</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12">
+      <c r="B38" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="G38" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="37">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I38" s="36">
         <v>1</v>
       </c>
-      <c r="J38" s="11">
+      <c r="J38" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K38" s="41"/>
+    </row>
+    <row r="39" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="40">
+        <f>A38+1</f>
+        <v>28</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="I39" s="36">
+        <v>1</v>
+      </c>
+      <c r="J39" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.13</v>
+      </c>
+      <c r="K39" s="41"/>
+    </row>
+    <row r="40" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
+        <f>A39+1</f>
+        <v>29</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="I40" s="12">
+        <v>1</v>
+      </c>
+      <c r="J40" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.26</v>
+      </c>
+      <c r="K40" s="13"/>
+    </row>
+    <row r="41" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="25">
+        <f t="shared" ref="A41:A44" si="2">A40+1</f>
+        <v>30</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H41" s="11">
+        <v>3.95</v>
+      </c>
+      <c r="I41" s="12">
+        <v>1</v>
+      </c>
+      <c r="J41" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.95</v>
+      </c>
+      <c r="K41" s="13"/>
+    </row>
+    <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12">
+        <v>1</v>
+      </c>
+      <c r="J42" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K38" s="13"/>
-    </row>
-    <row r="39" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A39" s="25">
-        <f>1+A38</f>
-        <v>28</v>
-      </c>
-      <c r="B39" s="10" t="s">
+      <c r="K42" s="13"/>
+    </row>
+    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H43" s="11"/>
+      <c r="I43" s="12">
+        <v>1</v>
+      </c>
+      <c r="J43" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="13"/>
+    </row>
+    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="11">
+        <v>1.04</v>
+      </c>
+      <c r="I44" s="12">
+        <v>4</v>
+      </c>
+      <c r="J44" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>4.16</v>
+      </c>
+      <c r="K44" s="13"/>
+    </row>
+    <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <f>A44+1</f>
+        <v>34</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="11">
+        <v>1.36</v>
+      </c>
+      <c r="I45" s="12">
+        <v>1</v>
+      </c>
+      <c r="J45" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.36</v>
+      </c>
+      <c r="K45" s="13"/>
+    </row>
+    <row r="46" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A46" s="25">
+        <f>A45+1</f>
+        <v>35</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="21" t="s">
+      <c r="F46" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="11">
+      <c r="G46" s="10"/>
+      <c r="H46" s="11">
         <v>150</v>
       </c>
-      <c r="I39" s="12">
+      <c r="I46" s="12">
         <v>1</v>
       </c>
-      <c r="J39" s="11">
+      <c r="J46" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>150</v>
       </c>
-      <c r="K39" s="13"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="11">
+      <c r="K46" s="13"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K40" s="13"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C42" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="K47" s="13"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="C49" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2931,12 +3409,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -2945,15 +3423,15 @@
         <v>7</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2966,7 +3444,7 @@
         <v>150</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote schematic and board layout version 2012. Added gerber files.
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="174">
   <si>
     <t>ID #</t>
   </si>
@@ -591,6 +591,15 @@
   </si>
   <si>
     <t>D1</t>
+  </si>
+  <si>
+    <t>BC2AAW-ND</t>
+  </si>
+  <si>
+    <t>BC2AAW</t>
+  </si>
+  <si>
+    <t>MPD (Memory Protection Devices)</t>
   </si>
 </sst>
 </file>
@@ -1890,8 +1899,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +1932,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>179.74</v>
+        <v>180.59</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -3168,9 +3177,7 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="21" t="s">
         <v>128</v>
@@ -3190,30 +3197,38 @@
       </c>
       <c r="K42" s="13"/>
     </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
+      <c r="B43" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="D43" s="21" t="s">
         <v>129</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="10"/>
+      <c r="F43" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="G43" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="11">
+        <v>0.85</v>
+      </c>
       <c r="I43" s="12">
         <v>1</v>
       </c>
       <c r="J43" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="K43" s="13"/>
     </row>

</xml_diff>

<commit_message>
Remote circuit - added reverse battery protection diode
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="19155" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="19155" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="179">
   <si>
     <t>ID #</t>
   </si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>3M</t>
-  </si>
-  <si>
-    <t>JP1</t>
   </si>
   <si>
     <t>Sparkfun</t>
@@ -600,6 +597,24 @@
   </si>
   <si>
     <t>MPD (Memory Protection Devices)</t>
+  </si>
+  <si>
+    <t>AVR</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>MBR0520L</t>
+  </si>
+  <si>
+    <t>Reverse battery protection diode</t>
+  </si>
+  <si>
+    <t>MBR0520LCT-ND</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -1584,8 +1599,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K47" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K48" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K48"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID #" dataDxfId="10">
       <calculatedColumnFormula>1+A2</calculatedColumnFormula>
@@ -1897,10 +1912,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1947,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>180.59</v>
+        <v>180.95</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -1991,6 +2006,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -2079,7 +2095,7 @@
         <v>56</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H6" s="29">
         <v>0.02</v>
@@ -2137,19 +2153,19 @@
         <v>52</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H8" s="37">
         <v>0.04</v>
@@ -2172,19 +2188,19 @@
         <v>52</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="H9" s="37">
         <v>0.04</v>
@@ -2234,7 +2250,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <f>A9+1</f>
+        <f>1+A9</f>
         <v>7</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -2244,13 +2260,13 @@
         <v>68</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>69</v>
@@ -2311,7 +2327,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>19</v>
@@ -2416,7 +2432,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>30</v>
@@ -2425,7 +2441,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>28</v>
@@ -2451,7 +2467,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>29</v>
@@ -2460,7 +2476,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>31</v>
@@ -2486,7 +2502,7 @@
         <v>65</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>32</v>
@@ -2495,7 +2511,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>33</v>
@@ -2556,19 +2572,19 @@
         <v>65</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H21" s="24">
         <v>0.38</v>
@@ -2588,22 +2604,22 @@
         <v>17</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>159</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>160</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>163</v>
       </c>
       <c r="H22" s="24">
         <v>7.0000000000000007E-2</v>
@@ -2765,19 +2781,19 @@
         <v>65</v>
       </c>
       <c r="C28" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>144</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="21" t="s">
         <v>145</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>146</v>
       </c>
       <c r="H28" s="35">
         <v>0.15</v>
@@ -2834,16 +2850,16 @@
         <v>80</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="21" t="s">
         <v>81</v>
@@ -2862,23 +2878,23 @@
     </row>
     <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
-        <f>A31+1</f>
+        <f>1+A31</f>
         <v>23</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E32" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>79</v>
@@ -2897,26 +2913,26 @@
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
-        <f>A32+1</f>
+        <f>1+A32</f>
         <v>24</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="34" t="s">
-        <v>124</v>
-      </c>
       <c r="D33" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="21" t="s">
         <v>125</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>126</v>
       </c>
       <c r="H33" s="35">
         <v>3.74</v>
@@ -2932,26 +2948,26 @@
     </row>
     <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
-        <f>A33+1</f>
+        <f>1+A33</f>
         <v>25</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H34" s="35">
         <v>3.17</v>
@@ -3036,26 +3052,26 @@
     </row>
     <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
-        <f>A37+1</f>
+        <f>1+A37</f>
         <v>27</v>
       </c>
       <c r="B38" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="D38" s="34" t="s">
         <v>167</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>168</v>
       </c>
       <c r="E38" s="43" t="s">
         <v>14</v>
       </c>
       <c r="F38" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="43" t="s">
         <v>169</v>
-      </c>
-      <c r="G38" s="43" t="s">
-        <v>170</v>
       </c>
       <c r="H38" s="37">
         <v>0.56999999999999995</v>
@@ -3071,7 +3087,7 @@
     </row>
     <row r="39" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
-        <f>A38+1</f>
+        <f>1+A38</f>
         <v>28</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -3105,185 +3121,195 @@
       <c r="K39" s="41"/>
     </row>
     <row r="40" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25">
-        <f>A39+1</f>
+      <c r="A40" s="40">
+        <f>1+A39</f>
         <v>29</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>92</v>
+      <c r="B40" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>175</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="10" t="s">
-        <v>93</v>
+      <c r="F40" s="43" t="s">
+        <v>177</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" s="11">
-        <v>0.26</v>
-      </c>
-      <c r="I40" s="12">
+        <v>178</v>
+      </c>
+      <c r="H40" s="37">
+        <v>0.36</v>
+      </c>
+      <c r="I40" s="36">
         <v>1</v>
       </c>
-      <c r="J40" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.26</v>
-      </c>
-      <c r="K40" s="13"/>
+      <c r="J40" s="37">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.36</v>
+      </c>
+      <c r="K40" s="41"/>
     </row>
     <row r="41" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25">
-        <f t="shared" ref="A41:A44" si="2">A40+1</f>
+        <f>1+A40</f>
         <v>30</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="10"/>
+        <v>95</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="D41" s="21" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="H41" s="11">
-        <v>3.95</v>
+        <v>0.26</v>
       </c>
       <c r="I41" s="12">
         <v>1</v>
       </c>
       <c r="J41" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.95</v>
+        <v>0.26</v>
       </c>
       <c r="K41" s="13"/>
     </row>
     <row r="42" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
-        <f t="shared" si="2"/>
+        <f>1+A41</f>
         <v>31</v>
       </c>
-      <c r="B42" s="10"/>
+      <c r="B42" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="C42" s="10"/>
       <c r="D42" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="11"/>
+        <v>96</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" s="11">
+        <v>3.95</v>
+      </c>
       <c r="I42" s="12">
         <v>1</v>
       </c>
       <c r="J42" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>3.95</v>
       </c>
       <c r="K42" s="13"/>
     </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
-        <f t="shared" si="2"/>
+        <f>1+A42</f>
         <v>32</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="C43" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="11">
+        <v>1.04</v>
+      </c>
+      <c r="I43" s="12">
+        <v>4</v>
+      </c>
+      <c r="J43" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>4.16</v>
+      </c>
+      <c r="K43" s="13"/>
+    </row>
+    <row r="44" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <f>1+A43</f>
+        <v>33</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="10" t="s">
+      <c r="C44" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="G43" s="10" t="s">
+      <c r="F44" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="G44" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H44" s="11">
         <v>0.85</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I44" s="12">
         <v>1</v>
       </c>
-      <c r="J43" s="11">
+      <c r="J44" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.85</v>
-      </c>
-      <c r="K43" s="13"/>
-    </row>
-    <row r="44" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="11">
-        <v>1.04</v>
-      </c>
-      <c r="I44" s="12">
-        <v>4</v>
-      </c>
-      <c r="J44" s="11">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>4.16</v>
       </c>
       <c r="K44" s="13"/>
     </row>
     <row r="45" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25">
-        <f>A44+1</f>
+        <f>1+A44</f>
         <v>34</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="11">
@@ -3298,72 +3324,90 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="46" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25">
-        <f>A45+1</f>
+        <f>1+A45</f>
         <v>35</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="11">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="13"/>
+    </row>
+    <row r="47" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A47" s="25">
+        <f>1+A46</f>
+        <v>36</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="21" t="s">
+      <c r="E47" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="F47" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F46" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G46" s="10"/>
-      <c r="H46" s="11">
+      <c r="G47" s="10"/>
+      <c r="H47" s="11">
         <v>150</v>
       </c>
-      <c r="I46" s="12">
+      <c r="I47" s="12">
         <v>1</v>
       </c>
-      <c r="J46" s="11">
+      <c r="J47" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>150</v>
       </c>
-      <c r="K46" s="13"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="11">
+      <c r="K47" s="13"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="11">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K47" s="13"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="K48" s="13"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
@@ -3375,7 +3419,8 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
@@ -3383,8 +3428,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
@@ -3397,6 +3441,11 @@
       <c r="A61" s="1"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3424,12 +3473,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -3438,15 +3487,15 @@
         <v>7</v>
       </c>
       <c r="D3" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -3459,7 +3508,7 @@
         <v>150</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wheelchair - functional LCD driver written
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="175">
   <si>
     <t>ID #</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>GPB507A05BR</t>
+  </si>
+  <si>
+    <t>throughhole: 1N5817-TPCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1918,8 +1921,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1937,7 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" style="32" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3126,7 +3129,7 @@
       </c>
       <c r="K39" s="40"/>
     </row>
-    <row r="40" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="39">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3159,7 +3162,9 @@
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.36</v>
       </c>
-      <c r="K40" s="40"/>
+      <c r="K40" s="37" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="41" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25">

</xml_diff>

<commit_message>
Wheelchair - LCD driver is now interrupt-driven
</commit_message>
<xml_diff>
--- a/hardware/Remote BOM.xlsx
+++ b/hardware/Remote BOM.xlsx
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>Cherry</t>
-  </si>
-  <si>
-    <t>MLZ2012M2R2H</t>
   </si>
   <si>
     <r>
@@ -400,9 +397,6 @@
     </r>
   </si>
   <si>
-    <t>445-8658-1-ND</t>
-  </si>
-  <si>
     <t>L4, L5</t>
   </si>
   <si>
@@ -623,6 +617,12 @@
   </si>
   <si>
     <t>throughhole: 1N5817-TPCT-ND</t>
+  </si>
+  <si>
+    <t>CPL2512T2R2M</t>
+  </si>
+  <si>
+    <t>445-4172-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1922,7 +1922,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="J1" s="28">
         <f>SUM(Table2[Sub Total])</f>
-        <v>32.04</v>
+        <v>32.64</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -2020,7 +2020,7 @@
         <v>49</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>37</v>
@@ -2052,19 +2052,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>55</v>
@@ -2102,7 +2102,7 @@
         <v>51</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H6" s="29">
         <v>0.02</v>
@@ -2125,16 +2125,16 @@
         <v>49</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>56</v>
@@ -2160,19 +2160,19 @@
         <v>49</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H8" s="36">
         <v>0.04</v>
@@ -2195,19 +2195,19 @@
         <v>49</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9" s="36">
         <v>0.04</v>
@@ -2267,7 +2267,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>14</v>
@@ -2429,7 +2429,7 @@
         <v>0.2</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2581,19 +2581,19 @@
         <v>58</v>
       </c>
       <c r="C21" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>133</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H21" s="24">
         <v>0.38</v>
@@ -2613,22 +2613,22 @@
         <v>17</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="D22" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H22" s="24">
         <v>7.0000000000000007E-2</v>
@@ -2790,29 +2790,29 @@
         <v>58</v>
       </c>
       <c r="C28" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>119</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>120</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H28" s="34">
-        <v>0.15</v>
+        <v>0.45</v>
       </c>
       <c r="I28" s="35">
         <v>2</v>
       </c>
       <c r="J28" s="36">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="K28" s="37"/>
     </row>
@@ -3065,22 +3065,22 @@
         <v>27</v>
       </c>
       <c r="B38" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="33" t="s">
         <v>142</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="D38" s="33" t="s">
-        <v>144</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>14</v>
       </c>
       <c r="F38" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G38" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H38" s="36">
         <v>0.56999999999999995</v>
@@ -3135,22 +3135,22 @@
         <v>29</v>
       </c>
       <c r="B40" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>151</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>153</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F40" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H40" s="36">
         <v>0.36</v>
@@ -3163,7 +3163,7 @@
         <v>0.36</v>
       </c>
       <c r="K40" s="37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3172,10 +3172,10 @@
         <v>30</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>85</v>
@@ -3184,10 +3184,10 @@
         <v>14</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H41" s="11">
         <v>0.28999999999999998</v>
@@ -3273,10 +3273,10 @@
         <v>33</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D44" s="21" t="s">
         <v>107</v>
@@ -3285,7 +3285,7 @@
         <v>14</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>79</v>
@@ -3311,7 +3311,7 @@
         <v>118</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>117</v>
@@ -3320,7 +3320,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="11">
@@ -3341,19 +3341,19 @@
         <v>35</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G46" s="42"/>
       <c r="H46" s="36">

</xml_diff>